<commit_message>
just specs now left
</commit_message>
<xml_diff>
--- a/TimeLineSasha.xlsx
+++ b/TimeLineSasha.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1989s\study\LastYear\Project\Assesment1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B686373A-9979-4168-A088-2A39C115D1C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D8BCA7-382F-447F-9C86-8F960524AFAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{812A7689-42C3-4291-B67A-7342A4DE46D2}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="74">
   <si>
     <t>Phase</t>
   </si>
@@ -235,9 +235,6 @@
   </si>
   <si>
     <t>Project Planner: Sasha Stepanov</t>
-  </si>
-  <si>
-    <t>Project Virtual prospection(draft)</t>
   </si>
   <si>
     <t>Create and identify Users</t>
@@ -298,6 +295,9 @@
       </rPr>
       <t>TBA</t>
     </r>
+  </si>
+  <si>
+    <t>Project FollowAra (draft)</t>
   </si>
 </sst>
 </file>
@@ -503,13 +503,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -801,26 +801,24 @@
   </sheetPr>
   <dimension ref="A1:K74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1640625" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.75" style="2" customWidth="1"/>
-    <col min="2" max="2" width="86.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.1640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="10.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="18.4140625" style="19" customWidth="1"/>
-    <col min="6" max="6" width="18.1640625" style="19" customWidth="1"/>
-    <col min="7" max="7" width="13.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="37.58203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="73.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17" style="19" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.83203125" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8.6640625" customWidth="1"/>
     <col min="9" max="16384" width="9.1640625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="28" x14ac:dyDescent="0.6">
       <c r="A1" s="11" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -848,7 +846,7 @@
     </row>
     <row r="3" spans="1:11" ht="18" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -862,7 +860,7 @@
     </row>
     <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -914,11 +912,11 @@
       <c r="K6" s="1"/>
     </row>
     <row r="7" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="30" t="s">
         <v>7</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C7" s="5">
         <v>1</v>
@@ -941,7 +939,7 @@
       <c r="K7" s="4"/>
     </row>
     <row r="8" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A8" s="29"/>
+      <c r="A8" s="30"/>
       <c r="B8" s="4" t="s">
         <v>8</v>
       </c>
@@ -958,7 +956,7 @@
         <v>44988</v>
       </c>
       <c r="G8" s="5">
-        <f t="shared" ref="G8:G71" si="0">C8-D8</f>
+        <f t="shared" ref="G8:G28" si="0">C8-D8</f>
         <v>0</v>
       </c>
       <c r="I8" s="4"/>
@@ -966,7 +964,7 @@
       <c r="K8" s="4"/>
     </row>
     <row r="9" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A9" s="29"/>
+      <c r="A9" s="30"/>
       <c r="B9" s="4" t="s">
         <v>9</v>
       </c>
@@ -991,7 +989,7 @@
       <c r="K9" s="4"/>
     </row>
     <row r="10" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A10" s="29"/>
+      <c r="A10" s="30"/>
       <c r="B10" s="4" t="s">
         <v>10</v>
       </c>
@@ -1016,7 +1014,7 @@
       <c r="K10" s="4"/>
     </row>
     <row r="11" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A11" s="29"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="4" t="s">
         <v>11</v>
       </c>
@@ -1025,10 +1023,10 @@
       </c>
       <c r="D11" s="5"/>
       <c r="E11" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="0"/>
@@ -1051,7 +1049,7 @@
       <c r="K12" s="4"/>
     </row>
     <row r="13" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="30" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="4" t="s">
@@ -1069,13 +1067,16 @@
       <c r="F13" s="15">
         <v>45000</v>
       </c>
-      <c r="G13" s="5"/>
+      <c r="G13" s="5">
+        <f>C13-D13</f>
+        <v>0</v>
+      </c>
       <c r="I13" s="4"/>
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
     </row>
     <row r="14" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A14" s="29"/>
+      <c r="A14" s="30"/>
       <c r="B14" s="4" t="s">
         <v>14</v>
       </c>
@@ -1091,13 +1092,16 @@
       <c r="F14" s="15">
         <v>45013</v>
       </c>
-      <c r="G14" s="5"/>
+      <c r="G14" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I14" s="4"/>
       <c r="J14" s="4"/>
       <c r="K14" s="4"/>
     </row>
     <row r="15" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A15" s="29"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="4" t="s">
         <v>15</v>
       </c>
@@ -1113,15 +1117,18 @@
       <c r="F15" s="15">
         <v>45000</v>
       </c>
-      <c r="G15" s="5"/>
+      <c r="G15" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.5</v>
+      </c>
       <c r="I15" s="4"/>
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
     </row>
     <row r="16" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A16" s="29"/>
+      <c r="A16" s="30"/>
       <c r="B16" s="12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C16" s="5">
         <v>1</v>
@@ -1135,13 +1142,16 @@
       <c r="F16" s="15">
         <v>45007</v>
       </c>
-      <c r="G16" s="5"/>
+      <c r="G16" s="5">
+        <f>C16-D16</f>
+        <v>-0.5</v>
+      </c>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
     </row>
     <row r="17" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A17" s="29"/>
+      <c r="A17" s="30"/>
       <c r="B17" s="12" t="s">
         <v>16</v>
       </c>
@@ -1157,13 +1167,16 @@
       <c r="F17" s="15">
         <v>45000</v>
       </c>
-      <c r="G17" s="5"/>
+      <c r="G17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
     </row>
     <row r="18" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A18" s="29"/>
+      <c r="A18" s="30"/>
       <c r="B18" s="4" t="s">
         <v>17</v>
       </c>
@@ -1179,13 +1192,16 @@
       <c r="F18" s="15">
         <v>45015</v>
       </c>
-      <c r="G18" s="5"/>
+      <c r="G18" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
     </row>
     <row r="19" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A19" s="29"/>
+      <c r="A19" s="30"/>
       <c r="B19" s="12" t="s">
         <v>56</v>
       </c>
@@ -1201,13 +1217,16 @@
       <c r="F19" s="15">
         <v>44990</v>
       </c>
-      <c r="G19" s="5"/>
+      <c r="G19" s="5">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
     </row>
     <row r="20" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A20" s="29"/>
+      <c r="A20" s="30"/>
       <c r="B20" s="4" t="s">
         <v>18</v>
       </c>
@@ -1223,13 +1242,16 @@
       <c r="F20" s="15">
         <v>45015</v>
       </c>
-      <c r="G20" s="5"/>
+      <c r="G20" s="5">
+        <f>C20-D20</f>
+        <v>-1</v>
+      </c>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
     </row>
     <row r="21" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A21" s="29"/>
+      <c r="A21" s="30"/>
       <c r="B21" s="12" t="s">
         <v>19</v>
       </c>
@@ -1245,13 +1267,16 @@
       <c r="F21" s="15">
         <v>45014</v>
       </c>
-      <c r="G21" s="5"/>
+      <c r="G21" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
     </row>
     <row r="22" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A22" s="29"/>
+      <c r="A22" s="30"/>
       <c r="B22" s="12" t="s">
         <v>20</v>
       </c>
@@ -1262,12 +1287,15 @@
         <v>3</v>
       </c>
       <c r="E22" s="15">
-        <v>45000</v>
-      </c>
-      <c r="F22" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G22" s="5"/>
+        <v>45031</v>
+      </c>
+      <c r="F22" s="15">
+        <v>45031</v>
+      </c>
+      <c r="G22" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
@@ -1285,45 +1313,59 @@
       <c r="K23" s="4"/>
     </row>
     <row r="24" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="30" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="F24" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G24" s="5"/>
+      <c r="C24" s="5">
+        <v>2</v>
+      </c>
+      <c r="D24" s="5">
+        <v>3</v>
+      </c>
+      <c r="E24" s="15">
+        <v>45018</v>
+      </c>
+      <c r="F24" s="15">
+        <v>45018</v>
+      </c>
+      <c r="G24" s="5">
+        <f t="shared" si="0"/>
+        <v>-1</v>
+      </c>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
     </row>
     <row r="25" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="29"/>
+      <c r="A25" s="30"/>
       <c r="B25" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="5"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="F25" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G25" s="5"/>
+      <c r="C25" s="5">
+        <v>1</v>
+      </c>
+      <c r="D25" s="5">
+        <v>1</v>
+      </c>
+      <c r="E25" s="15">
+        <v>45018</v>
+      </c>
+      <c r="F25" s="15">
+        <v>45018</v>
+      </c>
+      <c r="G25" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
     </row>
     <row r="26" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A26" s="29"/>
+      <c r="A26" s="30"/>
       <c r="B26" s="4" t="s">
         <v>24</v>
       </c>
@@ -1333,19 +1375,22 @@
       <c r="D26" s="5">
         <v>2</v>
       </c>
-      <c r="E26" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="F26" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G26" s="5"/>
+      <c r="E26" s="15">
+        <v>45018</v>
+      </c>
+      <c r="F26" s="15">
+        <v>45018</v>
+      </c>
+      <c r="G26" s="5">
+        <f>C26-D26</f>
+        <v>0</v>
+      </c>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
     </row>
     <row r="27" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A27" s="29"/>
+      <c r="A27" s="30"/>
       <c r="B27" s="4" t="s">
         <v>25</v>
       </c>
@@ -1355,19 +1400,22 @@
       <c r="D27" s="5">
         <v>1.5</v>
       </c>
-      <c r="E27" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="F27" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G27" s="5"/>
+      <c r="E27" s="15">
+        <v>45018</v>
+      </c>
+      <c r="F27" s="15">
+        <v>45018</v>
+      </c>
+      <c r="G27" s="5">
+        <f t="shared" si="0"/>
+        <v>-0.5</v>
+      </c>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
     </row>
     <row r="28" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A28" s="29"/>
+      <c r="A28" s="30"/>
       <c r="B28" s="4" t="s">
         <v>26</v>
       </c>
@@ -1377,13 +1425,16 @@
       <c r="D28" s="5">
         <v>2</v>
       </c>
-      <c r="E28" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="G28" s="5"/>
+      <c r="E28" s="15">
+        <v>45000</v>
+      </c>
+      <c r="F28" s="15">
+        <v>45000</v>
+      </c>
+      <c r="G28" s="5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -1401,7 +1452,7 @@
       <c r="K29" s="4"/>
     </row>
     <row r="30" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="30" t="s">
         <v>27</v>
       </c>
       <c r="B30" s="12" t="s">
@@ -1412,10 +1463,10 @@
       </c>
       <c r="D30" s="5"/>
       <c r="E30" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F30" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G30" s="5"/>
       <c r="H30" s="25"/>
@@ -1424,7 +1475,7 @@
       <c r="K30" s="25"/>
     </row>
     <row r="31" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A31" s="29"/>
+      <c r="A31" s="30"/>
       <c r="B31" s="4" t="s">
         <v>29</v>
       </c>
@@ -1433,10 +1484,10 @@
       </c>
       <c r="D31" s="5"/>
       <c r="E31" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G31" s="5"/>
       <c r="I31" s="4"/>
@@ -1444,7 +1495,7 @@
       <c r="K31" s="4"/>
     </row>
     <row r="32" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A32" s="29"/>
+      <c r="A32" s="30"/>
       <c r="B32" s="12" t="s">
         <v>30</v>
       </c>
@@ -1453,10 +1504,10 @@
       </c>
       <c r="D32" s="5"/>
       <c r="E32" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G32" s="5"/>
       <c r="I32" s="4"/>
@@ -1464,7 +1515,7 @@
       <c r="K32" s="4"/>
     </row>
     <row r="33" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A33" s="29"/>
+      <c r="A33" s="30"/>
       <c r="B33" s="4" t="s">
         <v>31</v>
       </c>
@@ -1473,10 +1524,10 @@
       </c>
       <c r="D33" s="5"/>
       <c r="E33" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G33" s="5"/>
       <c r="I33" s="4"/>
@@ -1484,7 +1535,7 @@
       <c r="K33" s="4"/>
     </row>
     <row r="34" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A34" s="29"/>
+      <c r="A34" s="30"/>
       <c r="B34" s="4" t="s">
         <v>32</v>
       </c>
@@ -1493,10 +1544,10 @@
       </c>
       <c r="D34" s="5"/>
       <c r="E34" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G34" s="5"/>
       <c r="I34" s="4"/>
@@ -1504,7 +1555,7 @@
       <c r="K34" s="4"/>
     </row>
     <row r="35" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A35" s="29"/>
+      <c r="A35" s="30"/>
       <c r="B35" s="4" t="s">
         <v>33</v>
       </c>
@@ -1513,10 +1564,10 @@
       </c>
       <c r="D35" s="5"/>
       <c r="E35" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G35" s="5"/>
       <c r="I35" s="4"/>
@@ -1524,7 +1575,7 @@
       <c r="K35" s="4"/>
     </row>
     <row r="36" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A36" s="29"/>
+      <c r="A36" s="30"/>
       <c r="B36" s="4" t="s">
         <v>34</v>
       </c>
@@ -1533,10 +1584,10 @@
       </c>
       <c r="D36" s="5"/>
       <c r="E36" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F36" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G36" s="5"/>
       <c r="I36" s="4"/>
@@ -1544,7 +1595,7 @@
       <c r="K36" s="4"/>
     </row>
     <row r="37" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A37" s="29"/>
+      <c r="A37" s="30"/>
       <c r="B37" s="12" t="s">
         <v>35</v>
       </c>
@@ -1553,10 +1604,10 @@
       </c>
       <c r="D37" s="5"/>
       <c r="E37" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F37" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G37" s="5"/>
       <c r="I37" s="4"/>
@@ -1564,17 +1615,17 @@
       <c r="K37" s="4"/>
     </row>
     <row r="38" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A38" s="29"/>
+      <c r="A38" s="30"/>
       <c r="B38" s="12" t="s">
         <v>57</v>
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="5"/>
       <c r="E38" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F38" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G38" s="5"/>
       <c r="I38" s="4"/>
@@ -1582,17 +1633,17 @@
       <c r="K38" s="4"/>
     </row>
     <row r="39" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A39" s="29"/>
+      <c r="A39" s="30"/>
       <c r="B39" s="12" t="s">
         <v>36</v>
       </c>
       <c r="C39" s="13"/>
       <c r="D39" s="28"/>
       <c r="E39" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F39" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G39" s="5"/>
       <c r="I39" s="1"/>
@@ -1612,7 +1663,7 @@
       <c r="K40" s="1"/>
     </row>
     <row r="41" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="30" t="s">
         <v>37</v>
       </c>
       <c r="B41" s="4" t="s">
@@ -1621,10 +1672,10 @@
       <c r="C41" s="28"/>
       <c r="D41" s="28"/>
       <c r="E41" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F41" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G41" s="5"/>
       <c r="I41" s="1"/>
@@ -1632,17 +1683,17 @@
       <c r="K41" s="1"/>
     </row>
     <row r="42" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A42" s="29"/>
+      <c r="A42" s="30"/>
       <c r="B42" s="4" t="s">
         <v>39</v>
       </c>
       <c r="C42" s="5"/>
       <c r="D42" s="5"/>
       <c r="E42" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F42" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G42" s="5"/>
       <c r="I42" s="1"/>
@@ -1650,17 +1701,17 @@
       <c r="K42" s="1"/>
     </row>
     <row r="43" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A43" s="29"/>
+      <c r="A43" s="30"/>
       <c r="B43" s="4" t="s">
         <v>31</v>
       </c>
       <c r="C43" s="5"/>
       <c r="D43" s="5"/>
       <c r="E43" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F43" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G43" s="5"/>
       <c r="I43" s="1"/>
@@ -1668,17 +1719,17 @@
       <c r="K43" s="1"/>
     </row>
     <row r="44" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A44" s="29"/>
+      <c r="A44" s="30"/>
       <c r="B44" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C44" s="5"/>
       <c r="D44" s="5"/>
       <c r="E44" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F44" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G44" s="5"/>
       <c r="I44" s="1"/>
@@ -1686,17 +1737,17 @@
       <c r="K44" s="1"/>
     </row>
     <row r="45" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A45" s="29"/>
+      <c r="A45" s="30"/>
       <c r="B45" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C45" s="5"/>
       <c r="D45" s="5"/>
       <c r="E45" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F45" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G45" s="5"/>
       <c r="I45" s="1"/>
@@ -1704,17 +1755,17 @@
       <c r="K45" s="1"/>
     </row>
     <row r="46" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A46" s="29"/>
+      <c r="A46" s="30"/>
       <c r="B46" s="4" t="s">
         <v>40</v>
       </c>
       <c r="C46" s="5"/>
       <c r="D46" s="5"/>
       <c r="E46" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F46" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G46" s="5"/>
       <c r="I46" s="1"/>
@@ -1734,7 +1785,7 @@
       <c r="K47" s="1"/>
     </row>
     <row r="48" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A48" s="29" t="s">
+      <c r="A48" s="30" t="s">
         <v>37</v>
       </c>
       <c r="B48" s="12" t="s">
@@ -1743,10 +1794,10 @@
       <c r="C48" s="5"/>
       <c r="D48" s="5"/>
       <c r="E48" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F48" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G48" s="5"/>
       <c r="I48" s="1"/>
@@ -1754,17 +1805,17 @@
       <c r="K48" s="1"/>
     </row>
     <row r="49" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A49" s="29"/>
+      <c r="A49" s="30"/>
       <c r="B49" s="12" t="s">
         <v>61</v>
       </c>
       <c r="C49" s="5"/>
       <c r="D49" s="5"/>
       <c r="E49" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F49" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G49" s="5"/>
       <c r="I49" s="1"/>
@@ -1784,7 +1835,7 @@
       <c r="K50" s="1"/>
     </row>
     <row r="51" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A51" s="29" t="s">
+      <c r="A51" s="30" t="s">
         <v>37</v>
       </c>
       <c r="B51" s="4" t="s">
@@ -1793,10 +1844,10 @@
       <c r="C51" s="5"/>
       <c r="D51" s="5"/>
       <c r="E51" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F51" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G51" s="5"/>
       <c r="I51" s="1"/>
@@ -1804,17 +1855,17 @@
       <c r="K51" s="1"/>
     </row>
     <row r="52" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A52" s="29"/>
+      <c r="A52" s="30"/>
       <c r="B52" s="4" t="s">
         <v>63</v>
       </c>
       <c r="C52" s="5"/>
       <c r="D52" s="5"/>
       <c r="E52" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F52" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G52" s="5"/>
       <c r="I52" s="1"/>
@@ -1822,17 +1873,17 @@
       <c r="K52" s="1"/>
     </row>
     <row r="53" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="29"/>
+      <c r="A53" s="30"/>
       <c r="B53" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C53" s="5"/>
       <c r="D53" s="5"/>
       <c r="E53" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F53" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G53" s="5"/>
       <c r="I53" s="1"/>
@@ -1840,17 +1891,17 @@
       <c r="K53" s="1"/>
     </row>
     <row r="54" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A54" s="29"/>
+      <c r="A54" s="30"/>
       <c r="B54" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C54" s="5"/>
       <c r="D54" s="5"/>
       <c r="E54" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F54" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G54" s="5"/>
       <c r="I54" s="1"/>
@@ -1858,17 +1909,17 @@
       <c r="K54" s="1"/>
     </row>
     <row r="55" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A55" s="29"/>
+      <c r="A55" s="30"/>
       <c r="B55" s="4" t="s">
         <v>64</v>
       </c>
       <c r="C55" s="5"/>
       <c r="D55" s="5"/>
       <c r="E55" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F55" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G55" s="5"/>
       <c r="I55" s="1"/>
@@ -1876,17 +1927,17 @@
       <c r="K55" s="1"/>
     </row>
     <row r="56" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A56" s="29"/>
+      <c r="A56" s="30"/>
       <c r="B56" s="4" t="s">
         <v>59</v>
       </c>
       <c r="C56" s="5"/>
       <c r="D56" s="5"/>
       <c r="E56" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F56" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G56" s="5"/>
       <c r="I56" s="1"/>
@@ -1894,17 +1945,17 @@
       <c r="K56" s="1"/>
     </row>
     <row r="57" spans="1:11" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A57" s="29"/>
+      <c r="A57" s="30"/>
       <c r="B57" s="14" t="s">
         <v>43</v>
       </c>
       <c r="C57" s="13"/>
       <c r="D57" s="28"/>
       <c r="E57" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F57" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G57" s="5"/>
       <c r="I57" s="1"/>
@@ -1924,7 +1975,7 @@
       <c r="K58" s="1"/>
     </row>
     <row r="59" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A59" s="30" t="s">
+      <c r="A59" s="31" t="s">
         <v>44</v>
       </c>
       <c r="B59" s="4" t="s">
@@ -1933,55 +1984,55 @@
       <c r="C59" s="5"/>
       <c r="D59" s="5"/>
       <c r="E59" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F59" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G59" s="5"/>
     </row>
     <row r="60" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A60" s="30"/>
+      <c r="A60" s="31"/>
       <c r="B60" s="4" t="s">
         <v>45</v>
       </c>
       <c r="C60" s="13"/>
       <c r="D60" s="13"/>
       <c r="E60" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F60" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G60" s="5"/>
     </row>
     <row r="61" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="30"/>
+      <c r="A61" s="31"/>
       <c r="B61" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C61" s="13"/>
       <c r="D61" s="28"/>
       <c r="E61" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F61" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G61" s="5"/>
     </row>
     <row r="62" spans="1:11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="30"/>
+      <c r="A62" s="31"/>
       <c r="B62" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C62" s="13"/>
       <c r="D62" s="28"/>
       <c r="E62" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F62" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G62" s="5"/>
       <c r="I62" s="2"/>
@@ -1989,17 +2040,17 @@
       <c r="K62" s="2"/>
     </row>
     <row r="63" spans="1:11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A63" s="30"/>
+      <c r="A63" s="31"/>
       <c r="B63" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C63" s="13"/>
       <c r="D63" s="28"/>
       <c r="E63" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F63" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G63" s="5"/>
       <c r="I63" s="2"/>
@@ -2007,17 +2058,17 @@
       <c r="K63" s="2"/>
     </row>
     <row r="64" spans="1:11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A64" s="30"/>
+      <c r="A64" s="31"/>
       <c r="B64" s="4" t="s">
         <v>65</v>
       </c>
       <c r="C64" s="13"/>
       <c r="D64" s="28"/>
       <c r="E64" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F64" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G64" s="5"/>
       <c r="I64" s="2"/>
@@ -2025,17 +2076,17 @@
       <c r="K64" s="2"/>
     </row>
     <row r="65" spans="1:11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="30"/>
+      <c r="A65" s="31"/>
       <c r="B65" s="4" t="s">
         <v>41</v>
       </c>
       <c r="C65" s="5"/>
       <c r="D65" s="5"/>
       <c r="E65" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F65" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G65" s="5"/>
       <c r="I65" s="2"/>
@@ -2043,17 +2094,17 @@
       <c r="K65" s="2"/>
     </row>
     <row r="66" spans="1:11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="30"/>
+      <c r="A66" s="31"/>
       <c r="B66" s="4" t="s">
         <v>49</v>
       </c>
       <c r="C66" s="13"/>
       <c r="D66" s="28"/>
       <c r="E66" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F66" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G66" s="5"/>
       <c r="I66" s="2"/>
@@ -2061,17 +2112,17 @@
       <c r="K66" s="2"/>
     </row>
     <row r="67" spans="1:11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A67" s="30"/>
+      <c r="A67" s="31"/>
       <c r="B67" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C67" s="13"/>
       <c r="D67" s="28"/>
       <c r="E67" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F67" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G67" s="5"/>
       <c r="I67" s="2"/>
@@ -2079,17 +2130,17 @@
       <c r="K67" s="2"/>
     </row>
     <row r="68" spans="1:11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A68" s="30"/>
+      <c r="A68" s="31"/>
       <c r="B68" s="4" t="s">
         <v>51</v>
       </c>
       <c r="C68" s="13"/>
       <c r="D68" s="28"/>
       <c r="E68" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F68" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G68" s="5"/>
       <c r="I68" s="2"/>
@@ -2097,17 +2148,17 @@
       <c r="K68" s="2"/>
     </row>
     <row r="69" spans="1:11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A69" s="30"/>
+      <c r="A69" s="31"/>
       <c r="B69" s="4" t="s">
         <v>52</v>
       </c>
       <c r="C69" s="13"/>
       <c r="D69" s="28"/>
       <c r="E69" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F69" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G69" s="5"/>
       <c r="I69" s="2"/>
@@ -2115,17 +2166,17 @@
       <c r="K69" s="2"/>
     </row>
     <row r="70" spans="1:11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="30"/>
+      <c r="A70" s="31"/>
       <c r="B70" s="9" t="s">
         <v>53</v>
       </c>
       <c r="C70" s="28"/>
       <c r="D70" s="28"/>
       <c r="E70" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F70" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G70" s="5"/>
       <c r="I70" s="2"/>
@@ -2151,11 +2202,11 @@
       </c>
       <c r="C72" s="8">
         <f>SUM(C7:C69)</f>
-        <v>41.5</v>
+        <v>44.5</v>
       </c>
       <c r="D72" s="8">
         <f>SUM(D7:D69)</f>
-        <v>26.9</v>
+        <v>30.9</v>
       </c>
       <c r="E72" s="18"/>
       <c r="F72" s="20" t="s">
@@ -2167,8 +2218,8 @@
       <c r="K72" s="2"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B74" s="31" t="s">
-        <v>70</v>
+      <c r="B74" s="29" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2197,12 +2248,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED5B6197DC005B418EDBAD81ECC78C65" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6af9fa09ccb0c32c90fa7665eb902fd5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="54363156-af09-451d-95c0-4bb150694616" xmlns:ns4="0588193f-5437-40c0-903e-14b41885f902" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3ada4b5171e24161cb51969d825ceddb" ns3:_="" ns4:_="">
     <xsd:import namespace="54363156-af09-451d-95c0-4bb150694616"/>
@@ -2419,6 +2464,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FD350447-97AF-434E-BC5F-409FF1FC1E65}">
   <ds:schemaRefs>
@@ -2428,23 +2479,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9761D45E-1D6F-403A-BC05-AA70C5A970CD}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="54363156-af09-451d-95c0-4bb150694616"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="0588193f-5437-40c0-903e-14b41885f902"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BE76EE25-C5C4-4176-B8D4-C72CCF8A1B82}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2461,4 +2495,21 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9761D45E-1D6F-403A-BC05-AA70C5A970CD}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="54363156-af09-451d-95c0-4bb150694616"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="0588193f-5437-40c0-903e-14b41885f902"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>